<commit_message>
Add top assists vs turnovers plot and head-to-head comparison tool
- Implemented `plot_top_assists_vs_turnovers` function to visualize assists vs turnovers with team logos and median lines.
- Created `generate_head_to_head_comparison` function for comparing two teams' statistics with visual representation.
- Added utility functions for logo extraction and color handling.
- Included example usage for both plotting functions in the main execution block.
</commit_message>
<xml_diff>
--- a/data/3FEB_25_26/assists_25_26_3FEB.xlsx
+++ b/data/3FEB_25_26/assists_25_26_3FEB.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1101"/>
+  <dimension ref="A1:G1209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36770,6 +36770,3570 @@
         <v>2</v>
       </c>
     </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1102" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1102" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1102" t="inlineStr">
+        <is>
+          <t>D. SHIELDS</t>
+        </is>
+      </c>
+      <c r="F1102" t="inlineStr">
+        <is>
+          <t>M. ESTAPE ROIZ</t>
+        </is>
+      </c>
+      <c r="G1102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1103" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1103" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="E1103" t="inlineStr">
+        <is>
+          <t>G. MARTIN LOPEZ-LAGO</t>
+        </is>
+      </c>
+      <c r="F1103" t="inlineStr">
+        <is>
+          <t>P. ROSSI</t>
+        </is>
+      </c>
+      <c r="G1103" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1104" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1104" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1104" t="inlineStr">
+        <is>
+          <t>M. ESTAPE ROIZ</t>
+        </is>
+      </c>
+      <c r="F1104" t="inlineStr">
+        <is>
+          <t>T. VERDERA BENASSAR</t>
+        </is>
+      </c>
+      <c r="G1104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1105" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1105" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1105" t="inlineStr">
+        <is>
+          <t>B. SCHUCH</t>
+        </is>
+      </c>
+      <c r="F1105" t="inlineStr">
+        <is>
+          <t>T. VERDERA BENASSAR</t>
+        </is>
+      </c>
+      <c r="G1105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1106" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1106" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1106" t="inlineStr">
+        <is>
+          <t>B. SCHUCH</t>
+        </is>
+      </c>
+      <c r="F1106" t="inlineStr">
+        <is>
+          <t>G. GOMA</t>
+        </is>
+      </c>
+      <c r="G1106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1107" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1107" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="E1107" t="inlineStr">
+        <is>
+          <t>A. GARCIA QUILEZ CUERVAS</t>
+        </is>
+      </c>
+      <c r="F1107" t="inlineStr">
+        <is>
+          <t>P. ROSSI</t>
+        </is>
+      </c>
+      <c r="G1107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1108" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1108" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1108" t="inlineStr">
+        <is>
+          <t>M. ESTAPE ROIZ</t>
+        </is>
+      </c>
+      <c r="F1108" t="inlineStr">
+        <is>
+          <t>F. MORENO GUTIERREZ</t>
+        </is>
+      </c>
+      <c r="G1108" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1109" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1109" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1109" t="inlineStr">
+        <is>
+          <t>G. FATA ALCARAZ</t>
+        </is>
+      </c>
+      <c r="F1109" t="inlineStr">
+        <is>
+          <t>T. PUNZANO VIEDMA</t>
+        </is>
+      </c>
+      <c r="G1109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1110" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1110" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="E1110" t="inlineStr">
+        <is>
+          <t>M. VILLAMANDOS TORRES</t>
+        </is>
+      </c>
+      <c r="F1110" t="inlineStr">
+        <is>
+          <t>C. CRESPO MONTESINOS</t>
+        </is>
+      </c>
+      <c r="G1110" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1111" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1111" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1111" t="inlineStr">
+        <is>
+          <t>T. PUNZANO VIEDMA</t>
+        </is>
+      </c>
+      <c r="F1111" t="inlineStr">
+        <is>
+          <t>L. SCHIEBELHUT LUIS</t>
+        </is>
+      </c>
+      <c r="G1111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1112" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1112" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="E1112" t="inlineStr">
+        <is>
+          <t>P. ROSSI</t>
+        </is>
+      </c>
+      <c r="F1112" t="inlineStr">
+        <is>
+          <t>S. PARADELA PARIS</t>
+        </is>
+      </c>
+      <c r="G1112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1113" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1113" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1113" t="inlineStr">
+        <is>
+          <t>T. VERDERA BENASSAR</t>
+        </is>
+      </c>
+      <c r="F1113" t="inlineStr">
+        <is>
+          <t>T. PUNZANO VIEDMA</t>
+        </is>
+      </c>
+      <c r="G1113" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1114" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1114" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1114" t="inlineStr">
+        <is>
+          <t>L. SCHIEBELHUT LUIS</t>
+        </is>
+      </c>
+      <c r="F1114" t="inlineStr">
+        <is>
+          <t>T. VERDERA BENASSAR</t>
+        </is>
+      </c>
+      <c r="G1114" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1115" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1115" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1115" t="inlineStr">
+        <is>
+          <t>J. VAQUERO PASCUAL</t>
+        </is>
+      </c>
+      <c r="F1115" t="inlineStr">
+        <is>
+          <t>L. SCHIEBELHUT LUIS</t>
+        </is>
+      </c>
+      <c r="G1115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1116" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1116" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="E1116" t="inlineStr">
+        <is>
+          <t>A. BIERSACK LOPEZ</t>
+        </is>
+      </c>
+      <c r="F1116" t="inlineStr">
+        <is>
+          <t>C. CRESPO MONTESINOS</t>
+        </is>
+      </c>
+      <c r="G1116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1117" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1117" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1117" t="inlineStr">
+        <is>
+          <t>J. VAQUERO PASCUAL</t>
+        </is>
+      </c>
+      <c r="F1117" t="inlineStr">
+        <is>
+          <t>M. RUBIO CORCHADO</t>
+        </is>
+      </c>
+      <c r="G1117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1118" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1118" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1118" t="inlineStr">
+        <is>
+          <t>G. FATA ALCARAZ</t>
+        </is>
+      </c>
+      <c r="F1118" t="inlineStr">
+        <is>
+          <t>M. RUBIO CORCHADO</t>
+        </is>
+      </c>
+      <c r="G1118" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1119" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1119" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1119" t="inlineStr">
+        <is>
+          <t>G. FATA ALCARAZ</t>
+        </is>
+      </c>
+      <c r="F1119" t="inlineStr">
+        <is>
+          <t>G. TCHIRAKADZE</t>
+        </is>
+      </c>
+      <c r="G1119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1120" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1120" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1120" t="inlineStr">
+        <is>
+          <t>B. SCHUCH</t>
+        </is>
+      </c>
+      <c r="F1120" t="inlineStr">
+        <is>
+          <t>L. SCHIEBELHUT LUIS</t>
+        </is>
+      </c>
+      <c r="G1120" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1121" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1121" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="E1121" t="inlineStr">
+        <is>
+          <t>A. BIERSACK LOPEZ</t>
+        </is>
+      </c>
+      <c r="F1121" t="inlineStr">
+        <is>
+          <t>G. MARTIN LOPEZ-LAGO</t>
+        </is>
+      </c>
+      <c r="G1121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1122" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1122" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="E1122" t="inlineStr">
+        <is>
+          <t>A. BIERSACK LOPEZ</t>
+        </is>
+      </c>
+      <c r="F1122" t="inlineStr">
+        <is>
+          <t>P. ESTEBANEZ GONZALEZ</t>
+        </is>
+      </c>
+      <c r="G1122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1123" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1123" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1123" t="inlineStr">
+        <is>
+          <t>B. SCHUCH</t>
+        </is>
+      </c>
+      <c r="F1123" t="inlineStr">
+        <is>
+          <t>T. PUNZANO VIEDMA</t>
+        </is>
+      </c>
+      <c r="G1123" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1124" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1124" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1124" t="inlineStr">
+        <is>
+          <t>J. VAQUERO PASCUAL</t>
+        </is>
+      </c>
+      <c r="F1124" t="inlineStr">
+        <is>
+          <t>M. ESTAPE ROIZ</t>
+        </is>
+      </c>
+      <c r="G1124" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1125" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1125" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="E1125" t="inlineStr">
+        <is>
+          <t>O. HADI ADEGBITE</t>
+        </is>
+      </c>
+      <c r="F1125" t="inlineStr">
+        <is>
+          <t>C. CRESPO MONTESINOS</t>
+        </is>
+      </c>
+      <c r="G1125" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1126" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1126" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1126" t="inlineStr">
+        <is>
+          <t>M. ESTAPE ROIZ</t>
+        </is>
+      </c>
+      <c r="F1126" t="inlineStr">
+        <is>
+          <t>G. GOMA</t>
+        </is>
+      </c>
+      <c r="G1126" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1127" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1127" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="E1127" t="inlineStr">
+        <is>
+          <t>G. MARTIN LOPEZ-LAGO</t>
+        </is>
+      </c>
+      <c r="F1127" t="inlineStr">
+        <is>
+          <t>D. MAGANTO LUCAS</t>
+        </is>
+      </c>
+      <c r="G1127" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1128" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1128" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="E1128" t="inlineStr">
+        <is>
+          <t>C. CRESPO MONTESINOS</t>
+        </is>
+      </c>
+      <c r="F1128" t="inlineStr">
+        <is>
+          <t>A. BIERSACK LOPEZ</t>
+        </is>
+      </c>
+      <c r="G1128" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1129" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1129" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1129" t="inlineStr">
+        <is>
+          <t>B. SCHUCH</t>
+        </is>
+      </c>
+      <c r="F1129" t="inlineStr">
+        <is>
+          <t>D. SHIELDS</t>
+        </is>
+      </c>
+      <c r="G1129" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1130" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1130" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS</t>
+        </is>
+      </c>
+      <c r="E1130" t="inlineStr">
+        <is>
+          <t>P. ESTEBANEZ GONZALEZ</t>
+        </is>
+      </c>
+      <c r="F1130" t="inlineStr">
+        <is>
+          <t>A. BIERSACK LOPEZ</t>
+        </is>
+      </c>
+      <c r="G1130" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1131" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>UROS DE RIVAS vs ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="D1131" t="inlineStr">
+        <is>
+          <t>ZENTRO BASKET MADRID</t>
+        </is>
+      </c>
+      <c r="E1131" t="inlineStr">
+        <is>
+          <t>B. SCHUCH</t>
+        </is>
+      </c>
+      <c r="F1131" t="inlineStr">
+        <is>
+          <t>M. RUBIO CORCHADO</t>
+        </is>
+      </c>
+      <c r="G1131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1132" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1132" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1132" t="inlineStr">
+        <is>
+          <t>M. DEL VALLE REGALADO</t>
+        </is>
+      </c>
+      <c r="F1132" t="inlineStr">
+        <is>
+          <t>S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="G1132" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1133" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1133" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1133" t="inlineStr">
+        <is>
+          <t>M. DEL VALLE REGALADO</t>
+        </is>
+      </c>
+      <c r="F1133" t="inlineStr">
+        <is>
+          <t>M. BATLLE BERNARDO</t>
+        </is>
+      </c>
+      <c r="G1133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1134" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1134" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1134" t="inlineStr">
+        <is>
+          <t>S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="F1134" t="inlineStr">
+        <is>
+          <t>M. BATLLE BERNARDO</t>
+        </is>
+      </c>
+      <c r="G1134" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1135" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1135" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="E1135" t="inlineStr">
+        <is>
+          <t>A. FERNÁNDEZ GÓMEZ</t>
+        </is>
+      </c>
+      <c r="F1135" t="inlineStr">
+        <is>
+          <t>A. REDONDO ALVAREZ DE SOTOMAYOR</t>
+        </is>
+      </c>
+      <c r="G1135" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1136" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1136" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1136" t="inlineStr">
+        <is>
+          <t>J. TRUJILLO FERNÁNDEZ</t>
+        </is>
+      </c>
+      <c r="F1136" t="inlineStr">
+        <is>
+          <t>D. TOLOSA OROPESA</t>
+        </is>
+      </c>
+      <c r="G1136" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1137" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1137" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1137" t="inlineStr">
+        <is>
+          <t>M. DEL VALLE REGALADO</t>
+        </is>
+      </c>
+      <c r="F1137" t="inlineStr">
+        <is>
+          <t>M. SANZ CÁMARA</t>
+        </is>
+      </c>
+      <c r="G1137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1138" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1138" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1138" t="inlineStr">
+        <is>
+          <t>S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="F1138" t="inlineStr">
+        <is>
+          <t>M. ALARCON ORTIZ</t>
+        </is>
+      </c>
+      <c r="G1138" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1139" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1139" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1139" t="inlineStr">
+        <is>
+          <t>C. BARROS CONDES</t>
+        </is>
+      </c>
+      <c r="F1139" t="inlineStr">
+        <is>
+          <t>M. ALARCON ORTIZ</t>
+        </is>
+      </c>
+      <c r="G1139" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1140" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1140" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1140" t="inlineStr">
+        <is>
+          <t>C. BARROS CONDES</t>
+        </is>
+      </c>
+      <c r="F1140" t="inlineStr">
+        <is>
+          <t>S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="G1140" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1141" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1141" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1141" t="inlineStr">
+        <is>
+          <t>F. SANTAMARIA LEON</t>
+        </is>
+      </c>
+      <c r="F1141" t="inlineStr">
+        <is>
+          <t>M. BATLLE BERNARDO</t>
+        </is>
+      </c>
+      <c r="G1141" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1142" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1142" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="E1142" t="inlineStr">
+        <is>
+          <t>A. MARTIN GONZALEZ</t>
+        </is>
+      </c>
+      <c r="F1142" t="inlineStr">
+        <is>
+          <t>A. FERNÁNDEZ GÓMEZ</t>
+        </is>
+      </c>
+      <c r="G1142" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1143" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1143" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1143" t="inlineStr">
+        <is>
+          <t>M. SANZ CÁMARA</t>
+        </is>
+      </c>
+      <c r="F1143" t="inlineStr">
+        <is>
+          <t>S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="G1143" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1144" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1144" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="E1144" t="inlineStr">
+        <is>
+          <t>P. SÁNCHEZ GUTIERREZ</t>
+        </is>
+      </c>
+      <c r="F1144" t="inlineStr">
+        <is>
+          <t>A. VIDAL RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="G1144" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1145" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1145" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1145" t="inlineStr">
+        <is>
+          <t>M. DEL VALLE REGALADO</t>
+        </is>
+      </c>
+      <c r="F1145" t="inlineStr">
+        <is>
+          <t>M. ALARCON ORTIZ</t>
+        </is>
+      </c>
+      <c r="G1145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1146" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1146" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="E1146" t="inlineStr">
+        <is>
+          <t>P. SÁNCHEZ GUTIERREZ</t>
+        </is>
+      </c>
+      <c r="F1146" t="inlineStr">
+        <is>
+          <t>A. REDONDO ALVAREZ DE SOTOMAYOR</t>
+        </is>
+      </c>
+      <c r="G1146" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1147" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1147" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1147" t="inlineStr">
+        <is>
+          <t>S. RODRIGUEZ GREGORIO</t>
+        </is>
+      </c>
+      <c r="F1147" t="inlineStr">
+        <is>
+          <t>L. BERMEJO ALCALDE</t>
+        </is>
+      </c>
+      <c r="G1147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1148" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1148" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1148" t="inlineStr">
+        <is>
+          <t>M. SANZ CÁMARA</t>
+        </is>
+      </c>
+      <c r="F1148" t="inlineStr">
+        <is>
+          <t>M. ALARCON ORTIZ</t>
+        </is>
+      </c>
+      <c r="G1148" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1149" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1149" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET</t>
+        </is>
+      </c>
+      <c r="E1149" t="inlineStr">
+        <is>
+          <t>M. ALARCON ORTIZ</t>
+        </is>
+      </c>
+      <c r="F1149" t="inlineStr">
+        <is>
+          <t>L. BERMEJO ALCALDE</t>
+        </is>
+      </c>
+      <c r="G1149" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1150" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>GRUPO EGIDO PINTOBASKET vs BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="D1150" t="inlineStr">
+        <is>
+          <t>BALONCESTO TELDE</t>
+        </is>
+      </c>
+      <c r="E1150" t="inlineStr">
+        <is>
+          <t>A. SANTANA OJEDA</t>
+        </is>
+      </c>
+      <c r="F1150" t="inlineStr">
+        <is>
+          <t>A. FERNÁNDEZ GÓMEZ</t>
+        </is>
+      </c>
+      <c r="G1150" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1151" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1151" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA</t>
+        </is>
+      </c>
+      <c r="E1151" t="inlineStr">
+        <is>
+          <t>P. RODRIGUEZ RIVERO</t>
+        </is>
+      </c>
+      <c r="F1151" t="inlineStr">
+        <is>
+          <t>O. PEÑA LOPEZ</t>
+        </is>
+      </c>
+      <c r="G1151" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1152" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1152" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="E1152" t="inlineStr">
+        <is>
+          <t>F. GOMEZ DE ENTERRIA LOPEZ</t>
+        </is>
+      </c>
+      <c r="F1152" t="inlineStr">
+        <is>
+          <t>A. SANCHO PEREZ</t>
+        </is>
+      </c>
+      <c r="G1152" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1153" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1153" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="E1153" t="inlineStr">
+        <is>
+          <t>J. ATIENZA PEREA</t>
+        </is>
+      </c>
+      <c r="F1153" t="inlineStr">
+        <is>
+          <t>N. MAIGA</t>
+        </is>
+      </c>
+      <c r="G1153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1154" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1154" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA</t>
+        </is>
+      </c>
+      <c r="E1154" t="inlineStr">
+        <is>
+          <t>D. OJEDA DAVILA</t>
+        </is>
+      </c>
+      <c r="F1154" t="inlineStr">
+        <is>
+          <t>I. REBERGEN</t>
+        </is>
+      </c>
+      <c r="G1154" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1155" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1155" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA</t>
+        </is>
+      </c>
+      <c r="E1155" t="inlineStr">
+        <is>
+          <t>D. RODRIGUEZ GARCIA</t>
+        </is>
+      </c>
+      <c r="F1155" t="inlineStr">
+        <is>
+          <t>O. PEÑA LOPEZ</t>
+        </is>
+      </c>
+      <c r="G1155" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1156" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1156" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="E1156" t="inlineStr">
+        <is>
+          <t>J. ATIENZA PEREA</t>
+        </is>
+      </c>
+      <c r="F1156" t="inlineStr">
+        <is>
+          <t>D. FERNANDEZ CAÑAS</t>
+        </is>
+      </c>
+      <c r="G1156" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1157" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1157" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA</t>
+        </is>
+      </c>
+      <c r="E1157" t="inlineStr">
+        <is>
+          <t>D. RODRIGUEZ GARCIA</t>
+        </is>
+      </c>
+      <c r="F1157" t="inlineStr">
+        <is>
+          <t>Y. RODRÍGUEZ MACHÍN</t>
+        </is>
+      </c>
+      <c r="G1157" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1158" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1158" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="E1158" t="inlineStr">
+        <is>
+          <t>J. ATIENZA PEREA</t>
+        </is>
+      </c>
+      <c r="F1158" t="inlineStr">
+        <is>
+          <t>F. GOMEZ DE ENTERRIA LOPEZ</t>
+        </is>
+      </c>
+      <c r="G1158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1159" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1159" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA</t>
+        </is>
+      </c>
+      <c r="E1159" t="inlineStr">
+        <is>
+          <t>E. GARCÍA PEREZ</t>
+        </is>
+      </c>
+      <c r="F1159" t="inlineStr">
+        <is>
+          <t>D. RODRIGUEZ GARCIA</t>
+        </is>
+      </c>
+      <c r="G1159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1160" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1160" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA</t>
+        </is>
+      </c>
+      <c r="E1160" t="inlineStr">
+        <is>
+          <t>D. RODRIGUEZ GARCIA</t>
+        </is>
+      </c>
+      <c r="F1160" t="inlineStr">
+        <is>
+          <t>M. NIANG</t>
+        </is>
+      </c>
+      <c r="G1160" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1161" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1161" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA</t>
+        </is>
+      </c>
+      <c r="E1161" t="inlineStr">
+        <is>
+          <t>I. REBERGEN</t>
+        </is>
+      </c>
+      <c r="F1161" t="inlineStr">
+        <is>
+          <t>M. NIANG</t>
+        </is>
+      </c>
+      <c r="G1161" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1162" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1162" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="E1162" t="inlineStr">
+        <is>
+          <t>D. GONZALEZ LONGARELA</t>
+        </is>
+      </c>
+      <c r="F1162" t="inlineStr">
+        <is>
+          <t>R. LARDIES GUILLEN</t>
+        </is>
+      </c>
+      <c r="G1162" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1163" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1163" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="E1163" t="inlineStr">
+        <is>
+          <t>D. GONZALEZ LONGARELA</t>
+        </is>
+      </c>
+      <c r="F1163" t="inlineStr">
+        <is>
+          <t>N. MAIGA</t>
+        </is>
+      </c>
+      <c r="G1163" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1164" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1164" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="E1164" t="inlineStr">
+        <is>
+          <t>N. MAIGA</t>
+        </is>
+      </c>
+      <c r="F1164" t="inlineStr">
+        <is>
+          <t>J. DOMINGUEZ LARRE</t>
+        </is>
+      </c>
+      <c r="G1164" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1165" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>C. D. MENSAJERO ISLA DE LA PALMA vs C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="D1165" t="inlineStr">
+        <is>
+          <t>C.B. TRES CANTOS</t>
+        </is>
+      </c>
+      <c r="E1165" t="inlineStr">
+        <is>
+          <t>A. SIMON DEL CORRAL</t>
+        </is>
+      </c>
+      <c r="F1165" t="inlineStr">
+        <is>
+          <t>D. GONZALEZ LONGARELA</t>
+        </is>
+      </c>
+      <c r="G1165" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1166" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1166" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="E1166" t="inlineStr">
+        <is>
+          <t>H. SANTANA DE LA ROSA</t>
+        </is>
+      </c>
+      <c r="F1166" t="inlineStr">
+        <is>
+          <t>E. PEREZ BERNABEU</t>
+        </is>
+      </c>
+      <c r="G1166" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1167" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1167" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="E1167" t="inlineStr">
+        <is>
+          <t>E. LLACER SIMLAT</t>
+        </is>
+      </c>
+      <c r="F1167" t="inlineStr">
+        <is>
+          <t>S. GUEYE</t>
+        </is>
+      </c>
+      <c r="G1167" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1168" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1168" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="E1168" t="inlineStr">
+        <is>
+          <t>S. GUEYE</t>
+        </is>
+      </c>
+      <c r="F1168" t="inlineStr">
+        <is>
+          <t>E. LLACER SIMLAT</t>
+        </is>
+      </c>
+      <c r="G1168" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1169" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1169" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="E1169" t="inlineStr">
+        <is>
+          <t>E. LLACER SIMLAT</t>
+        </is>
+      </c>
+      <c r="F1169" t="inlineStr">
+        <is>
+          <t>A. JIMÉNEZ BARRETO</t>
+        </is>
+      </c>
+      <c r="G1169" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1170" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1170" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="E1170" t="inlineStr">
+        <is>
+          <t>O. BALSELLS PLAZA</t>
+        </is>
+      </c>
+      <c r="F1170" t="inlineStr">
+        <is>
+          <t>D. VIERA LOPEZ</t>
+        </is>
+      </c>
+      <c r="G1170" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1171" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1171" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="E1171" t="inlineStr">
+        <is>
+          <t>O. BALSELLS PLAZA</t>
+        </is>
+      </c>
+      <c r="F1171" t="inlineStr">
+        <is>
+          <t>K. SKUTYELNIK</t>
+        </is>
+      </c>
+      <c r="G1171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1172" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1172" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="E1172" t="inlineStr">
+        <is>
+          <t>A. OLMEDO VELASCO</t>
+        </is>
+      </c>
+      <c r="F1172" t="inlineStr">
+        <is>
+          <t>I. BLANCO-ARGIBAY GONZALEZ</t>
+        </is>
+      </c>
+      <c r="G1172" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1173" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1173" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="E1173" t="inlineStr">
+        <is>
+          <t>S. KONE</t>
+        </is>
+      </c>
+      <c r="F1173" t="inlineStr">
+        <is>
+          <t>A. JIMÉNEZ BARRETO</t>
+        </is>
+      </c>
+      <c r="G1173" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1174" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1174" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="E1174" t="inlineStr">
+        <is>
+          <t>I. BLANCO-ARGIBAY GONZALEZ</t>
+        </is>
+      </c>
+      <c r="F1174" t="inlineStr">
+        <is>
+          <t>C. CUESTA DE SANTOS</t>
+        </is>
+      </c>
+      <c r="G1174" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1175" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1175" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="E1175" t="inlineStr">
+        <is>
+          <t>C. CUESTA DE SANTOS</t>
+        </is>
+      </c>
+      <c r="F1175" t="inlineStr">
+        <is>
+          <t>A. OLMEDO VELASCO</t>
+        </is>
+      </c>
+      <c r="G1175" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1176" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1176" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="E1176" t="inlineStr">
+        <is>
+          <t>J. ABRIL RAMIRO</t>
+        </is>
+      </c>
+      <c r="F1176" t="inlineStr">
+        <is>
+          <t>S. GUEYE</t>
+        </is>
+      </c>
+      <c r="G1176" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1177" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1177" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="E1177" t="inlineStr">
+        <is>
+          <t>A. JIMÉNEZ BARRETO</t>
+        </is>
+      </c>
+      <c r="F1177" t="inlineStr">
+        <is>
+          <t>D. VIERA LOPEZ</t>
+        </is>
+      </c>
+      <c r="G1177" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1178" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1178" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="E1178" t="inlineStr">
+        <is>
+          <t>K. SKUTYELNIK</t>
+        </is>
+      </c>
+      <c r="F1178" t="inlineStr">
+        <is>
+          <t>S. KONE</t>
+        </is>
+      </c>
+      <c r="G1178" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1179" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1179" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="E1179" t="inlineStr">
+        <is>
+          <t>I. BLANCO-ARGIBAY GONZALEZ</t>
+        </is>
+      </c>
+      <c r="F1179" t="inlineStr">
+        <is>
+          <t>H. SANTANA DE LA ROSA</t>
+        </is>
+      </c>
+      <c r="G1179" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1180" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1180" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="E1180" t="inlineStr">
+        <is>
+          <t>J. LARREA IBARBURU</t>
+        </is>
+      </c>
+      <c r="F1180" t="inlineStr">
+        <is>
+          <t>J. ABRIL RAMIRO</t>
+        </is>
+      </c>
+      <c r="G1180" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1181" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1181" t="inlineStr">
+        <is>
+          <t>ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="E1181" t="inlineStr">
+        <is>
+          <t>E. BOADA MONTESDEOCA</t>
+        </is>
+      </c>
+      <c r="F1181" t="inlineStr">
+        <is>
+          <t>H. SANTANA DE LA ROSA</t>
+        </is>
+      </c>
+      <c r="G1181" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1182" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>CB ARIDANE vs ADC BOADILLA</t>
+        </is>
+      </c>
+      <c r="D1182" t="inlineStr">
+        <is>
+          <t>CB ARIDANE</t>
+        </is>
+      </c>
+      <c r="E1182" t="inlineStr">
+        <is>
+          <t>D. VIERA LOPEZ</t>
+        </is>
+      </c>
+      <c r="F1182" t="inlineStr">
+        <is>
+          <t>J. ABRIL RAMIRO</t>
+        </is>
+      </c>
+      <c r="G1182" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1183" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1183" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1183" t="inlineStr">
+        <is>
+          <t>E. PASCUAL COZAR</t>
+        </is>
+      </c>
+      <c r="F1183" t="inlineStr">
+        <is>
+          <t>M. HERMOSO ALCUBILLA</t>
+        </is>
+      </c>
+      <c r="G1183" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1184" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1184" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1184" t="inlineStr">
+        <is>
+          <t>E. PASCUAL COZAR</t>
+        </is>
+      </c>
+      <c r="F1184" t="inlineStr">
+        <is>
+          <t>J. LAPASTORA ARACIL</t>
+        </is>
+      </c>
+      <c r="G1184" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1185" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1185" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1185" t="inlineStr">
+        <is>
+          <t>E. PASCUAL COZAR</t>
+        </is>
+      </c>
+      <c r="F1185" t="inlineStr">
+        <is>
+          <t>N. LASUNCION MARIBLANCA</t>
+        </is>
+      </c>
+      <c r="G1185" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1186" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1186" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1186" t="inlineStr">
+        <is>
+          <t>N. LASUNCION MARIBLANCA</t>
+        </is>
+      </c>
+      <c r="F1186" t="inlineStr">
+        <is>
+          <t>E. PASCUAL COZAR</t>
+        </is>
+      </c>
+      <c r="G1186" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1187" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1187" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="E1187" t="inlineStr">
+        <is>
+          <t>C. KLOTZ MAROTO</t>
+        </is>
+      </c>
+      <c r="F1187" t="inlineStr">
+        <is>
+          <t>B. GUEYE</t>
+        </is>
+      </c>
+      <c r="G1187" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1188" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1188" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1188" t="inlineStr">
+        <is>
+          <t>M. HERMOSO ALCUBILLA</t>
+        </is>
+      </c>
+      <c r="F1188" t="inlineStr">
+        <is>
+          <t>N. LASUNCION MARIBLANCA</t>
+        </is>
+      </c>
+      <c r="G1188" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1189" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1189" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="E1189" t="inlineStr">
+        <is>
+          <t>A. VICENTE VIANA</t>
+        </is>
+      </c>
+      <c r="F1189" t="inlineStr">
+        <is>
+          <t>V. ALONSO PASCUAL</t>
+        </is>
+      </c>
+      <c r="G1189" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1190" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1190" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1190" t="inlineStr">
+        <is>
+          <t>J. GARCIA-LARRACHE SEGURA</t>
+        </is>
+      </c>
+      <c r="F1190" t="inlineStr">
+        <is>
+          <t>N. LASUNCION MARIBLANCA</t>
+        </is>
+      </c>
+      <c r="G1190" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1191" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1191" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1191" t="inlineStr">
+        <is>
+          <t>L. GARCIA LARRACHE SEGURA</t>
+        </is>
+      </c>
+      <c r="F1191" t="inlineStr">
+        <is>
+          <t>D. MANZANERO CAMACHO</t>
+        </is>
+      </c>
+      <c r="G1191" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1192" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1192" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="E1192" t="inlineStr">
+        <is>
+          <t>A. VICENTE VIANA</t>
+        </is>
+      </c>
+      <c r="F1192" t="inlineStr">
+        <is>
+          <t>C. KLOTZ MAROTO</t>
+        </is>
+      </c>
+      <c r="G1192" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1193" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1193" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="E1193" t="inlineStr">
+        <is>
+          <t>A. VICENTE VIANA</t>
+        </is>
+      </c>
+      <c r="F1193" t="inlineStr">
+        <is>
+          <t>C. UNANUE CEGARRA</t>
+        </is>
+      </c>
+      <c r="G1193" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1194" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1194" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1194" t="inlineStr">
+        <is>
+          <t>D. MANZANERO CAMACHO</t>
+        </is>
+      </c>
+      <c r="F1194" t="inlineStr">
+        <is>
+          <t>L. GARCIA LARRACHE SEGURA</t>
+        </is>
+      </c>
+      <c r="G1194" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1195" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1195" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="E1195" t="inlineStr">
+        <is>
+          <t>C. KLOTZ MAROTO</t>
+        </is>
+      </c>
+      <c r="F1195" t="inlineStr">
+        <is>
+          <t>C. UNANUE CEGARRA</t>
+        </is>
+      </c>
+      <c r="G1195" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1196" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1196" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1196" t="inlineStr">
+        <is>
+          <t>M. KREISLER LORENTE</t>
+        </is>
+      </c>
+      <c r="F1196" t="inlineStr">
+        <is>
+          <t>J. OLIVA SANCHEZ</t>
+        </is>
+      </c>
+      <c r="G1196" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1197" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1197" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="E1197" t="inlineStr">
+        <is>
+          <t>D. LORENZO NEGRETE</t>
+        </is>
+      </c>
+      <c r="F1197" t="inlineStr">
+        <is>
+          <t>C. UNANUE CEGARRA</t>
+        </is>
+      </c>
+      <c r="G1197" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1198" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1198" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1198" t="inlineStr">
+        <is>
+          <t>J. OLIVA SANCHEZ</t>
+        </is>
+      </c>
+      <c r="F1198" t="inlineStr">
+        <is>
+          <t>E. MARTINEZ ALVAREZ</t>
+        </is>
+      </c>
+      <c r="G1198" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1199" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1199" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="E1199" t="inlineStr">
+        <is>
+          <t>D. LORENZO NEGRETE</t>
+        </is>
+      </c>
+      <c r="F1199" t="inlineStr">
+        <is>
+          <t>A. VICENTE VIANA</t>
+        </is>
+      </c>
+      <c r="G1199" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1200" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1200" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="E1200" t="inlineStr">
+        <is>
+          <t>B. GUEYE</t>
+        </is>
+      </c>
+      <c r="F1200" t="inlineStr">
+        <is>
+          <t>A. VICENTE VIANA</t>
+        </is>
+      </c>
+      <c r="G1200" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1201" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1201" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1201" t="inlineStr">
+        <is>
+          <t>E. PASCUAL COZAR</t>
+        </is>
+      </c>
+      <c r="F1201" t="inlineStr">
+        <is>
+          <t>D. MANZANERO CAMACHO</t>
+        </is>
+      </c>
+      <c r="G1201" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1202" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1202" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1202" t="inlineStr">
+        <is>
+          <t>E. MARTINEZ ALVAREZ</t>
+        </is>
+      </c>
+      <c r="F1202" t="inlineStr">
+        <is>
+          <t>D. MANZANERO CAMACHO</t>
+        </is>
+      </c>
+      <c r="G1202" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1203" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1203" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1203" t="inlineStr">
+        <is>
+          <t>J. LAPASTORA ARACIL</t>
+        </is>
+      </c>
+      <c r="F1203" t="inlineStr">
+        <is>
+          <t>E. PASCUAL COZAR</t>
+        </is>
+      </c>
+      <c r="G1203" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1204" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1204" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1204" t="inlineStr">
+        <is>
+          <t>J. GARCIA-LARRACHE SEGURA</t>
+        </is>
+      </c>
+      <c r="F1204" t="inlineStr">
+        <is>
+          <t>J. LAPASTORA ARACIL</t>
+        </is>
+      </c>
+      <c r="G1204" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1205" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1205" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1205" t="inlineStr">
+        <is>
+          <t>J. LAPASTORA ARACIL</t>
+        </is>
+      </c>
+      <c r="F1205" t="inlineStr">
+        <is>
+          <t>J. GARCIA-LARRACHE SEGURA</t>
+        </is>
+      </c>
+      <c r="G1205" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1206" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1206" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="E1206" t="inlineStr">
+        <is>
+          <t>C. UNANUE CEGARRA</t>
+        </is>
+      </c>
+      <c r="F1206" t="inlineStr">
+        <is>
+          <t>V. ALONSO PASCUAL</t>
+        </is>
+      </c>
+      <c r="G1206" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1207" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1207" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="E1207" t="inlineStr">
+        <is>
+          <t>D. LORENZO NEGRETE</t>
+        </is>
+      </c>
+      <c r="F1207" t="inlineStr">
+        <is>
+          <t>V. ALONSO PASCUAL</t>
+        </is>
+      </c>
+      <c r="G1207" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1208" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1208" t="inlineStr">
+        <is>
+          <t>BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="E1208" t="inlineStr">
+        <is>
+          <t>D. LORENZO NEGRETE</t>
+        </is>
+      </c>
+      <c r="F1208" t="inlineStr">
+        <is>
+          <t>M. BALDAN MARTÍN</t>
+        </is>
+      </c>
+      <c r="G1208" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>Liga Regular "B-B"</t>
+        </is>
+      </c>
+      <c r="B1209" t="n">
+        <v>8</v>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C. vs BALONCESTO TALAVERA</t>
+        </is>
+      </c>
+      <c r="D1209" t="inlineStr">
+        <is>
+          <t>REAL CANOE N.C.</t>
+        </is>
+      </c>
+      <c r="E1209" t="inlineStr">
+        <is>
+          <t>D. MANZANERO CAMACHO</t>
+        </is>
+      </c>
+      <c r="F1209" t="inlineStr">
+        <is>
+          <t>E. MARTINEZ ALVAREZ</t>
+        </is>
+      </c>
+      <c r="G1209" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>